<commit_message>
split timesheets to own workbook
</commit_message>
<xml_diff>
--- a/contract_management/spec/support/test_files/bookkeeping/contracts.xlsx
+++ b/contract_management/spec/support/test_files/bookkeeping/contracts.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/f3m-mbp1/dev/f3mmedia/accounts_tools/contract_management/spec/support/source_test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/f3m-mbp1/dev/f3mmedia/accounts_tools/contract_management/spec/support/test_files/bookkeeping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A47DDCD-7612-A748-AC43-9DDCA70A97FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B36B11-EDAA-2C4B-96AD-E4B0EF991536}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35740" yWindow="1940" windowWidth="26840" windowHeight="14500" activeTab="1" xr2:uid="{F6BEFC03-07BC-4145-8443-7E8EFAFFA442}"/>
+    <workbookView xWindow="35740" yWindow="1940" windowWidth="26840" windowHeight="14500" xr2:uid="{F6BEFC03-07BC-4145-8443-7E8EFAFFA442}"/>
   </bookViews>
   <sheets>
-    <sheet name="timesheets" sheetId="1" r:id="rId1"/>
-    <sheet name="contracts" sheetId="2" r:id="rId2"/>
+    <sheet name="contracts" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,25 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
-  <si>
-    <t>1-1</t>
-  </si>
-  <si>
-    <t>days</t>
-  </si>
-  <si>
-    <t>timesheet</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>period</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -59,9 +40,6 @@
   </si>
   <si>
     <t>rate</t>
-  </si>
-  <si>
-    <t>some_customer</t>
   </si>
   <si>
     <t>some_client</t>
@@ -71,26 +49,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -101,7 +66,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,18 +75,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -129,54 +88,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -492,89 +418,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE01397C-AA72-3A49-A727-2D5401A5CDDC}">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="E2" sqref="E2"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>40424</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>40427</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B8E2DE-E58D-F449-80B1-093E79C803C4}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -585,25 +428,25 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="11"/>
-    <col min="5" max="5" width="10.83203125" style="12"/>
+    <col min="3" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>10</v>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -611,15 +454,15 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="11">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
         <v>40422</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="1">
         <v>40548</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="2">
         <v>100</v>
       </c>
     </row>
@@ -628,15 +471,15 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="11">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
         <v>40778</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="1">
         <v>40998</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="2">
         <v>100</v>
       </c>
     </row>

</xml_diff>